<commit_message>
Bayesian ridge, Gradient boost and SVR methods throw the same error because they expect a 1D output array. In our case, the array is have a size of 6 along axis 1
</commit_message>
<xml_diff>
--- a/FT_reaction_ML_project/catalyst_performance_optimizer/properties.xlsx
+++ b/FT_reaction_ML_project/catalyst_performance_optimizer/properties.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/hiregangea_cardiff_ac_uk/Documents/Desktop/personal_projects/FT_reaction_ML_project/experimental_optimizing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/hiregangea_cardiff_ac_uk/Documents/Desktop/personal_projects/FT_reaction_ML_project/catalyst_performance_optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC104873399A41685BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{975DF1E2-EBDA-49CC-A9AB-2688A17C849D}"/>
@@ -131,6 +131,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,7 +403,7 @@
   <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>